<commit_message>
Continuando a formatação de impresão
</commit_message>
<xml_diff>
--- a/EXCEL/obras_2021.xlsx
+++ b/EXCEL/obras_2021.xlsx
@@ -5,20 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan.pinto\Desktop\Códigos\Projeto - Controle de obras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan.pinto\Desktop\Códigos\Projeto - Controle de obras\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7EF48D-761D-4A06-B979-2A6051D2E955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35748F1-C8F0-40FF-98E9-7B0FEFBE893B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="24000" windowHeight="13050" activeTab="2" xr2:uid="{4E9D2131-4700-4170-8715-5454C4ACF7F8}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="24000" windowHeight="13050" xr2:uid="{4E9D2131-4700-4170-8715-5454C4ACF7F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="format" sheetId="2" r:id="rId2"/>
-    <sheet name="mod imp inventario" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">format!$A$1:$N$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$N$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
   <si>
     <t>OBJETO</t>
   </si>
@@ -298,111 +295,6 @@
   </si>
   <si>
     <t>PARADA TÉCNICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000000 </t>
-  </si>
-  <si>
-    <t>15451001410950000</t>
-  </si>
-  <si>
-    <t>27101</t>
-  </si>
-  <si>
-    <t>44905117</t>
-  </si>
-  <si>
-    <t>U.O.</t>
-  </si>
-  <si>
-    <t>123210517</t>
-  </si>
-  <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>TIPO</t>
-  </si>
-  <si>
-    <t>Empenho</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nr. Contrato:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 018/2021</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vlr. do Contrato:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 271.269,96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Status:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> PARADA TÉCNICA</t>
-    </r>
-  </si>
-  <si>
-    <t>Obra:</t>
-  </si>
-  <si>
-    <t>Empresa/Credor:</t>
-  </si>
-  <si>
-    <t>NATUREZA / C. CONTÁBIL</t>
-  </si>
-  <si>
-    <t>PT / 
-FONTE</t>
   </si>
 </sst>
 </file>
@@ -414,7 +306,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,84 +356,6 @@
       <color rgb="FFC00000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -600,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -820,35 +634,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -859,7 +644,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1058,304 +843,6 @@
     </xf>
     <xf numFmtId="44" fontId="5" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="7" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="9" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="9" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="7" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="7" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="8" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="8" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1677,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B109D0-669A-4E04-8027-327E3EF3F49B}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -2502,1053 +1989,4 @@
   <autoFilter ref="A1:N20" xr:uid="{80B109D0-669A-4E04-8027-327E3EF3F49B}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8D3DC1-D94F-4F8A-A51F-5D1DAD8FBFB5}">
-  <dimension ref="A1:N28"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="119.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.28515625" style="67" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="67"/>
-    <col min="4" max="4" width="22.5703125" style="67" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="67" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="67" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="67"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="73" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="74" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="77">
-        <v>271269.96000000002</v>
-      </c>
-      <c r="F2" s="77">
-        <v>271269.96000000002</v>
-      </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="80" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="82" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="89"/>
-    </row>
-    <row r="4" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="89"/>
-    </row>
-    <row r="5" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="89"/>
-    </row>
-    <row r="7" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="73" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="80" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="82" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="74" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="77">
-        <v>271269.96000000002</v>
-      </c>
-      <c r="F11" s="90"/>
-      <c r="G11" s="91">
-        <v>32509.05</v>
-      </c>
-      <c r="H11" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="93" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="94" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="80" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="98" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="99" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="100">
-        <v>4465537.18</v>
-      </c>
-      <c r="F12" s="100">
-        <v>4465537.18</v>
-      </c>
-      <c r="G12" s="101"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="98" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="99" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="100">
-        <v>4465537.18</v>
-      </c>
-      <c r="F13" s="103"/>
-      <c r="G13" s="104">
-        <v>39791.08</v>
-      </c>
-      <c r="H13" s="105"/>
-      <c r="I13" s="106" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="107" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="108" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="109">
-        <v>374643.14</v>
-      </c>
-      <c r="F14" s="110">
-        <v>347643.14</v>
-      </c>
-      <c r="G14" s="110"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="97" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="107" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="108" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="109">
-        <v>374643.14</v>
-      </c>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91">
-        <v>77471.25</v>
-      </c>
-      <c r="H15" s="111"/>
-      <c r="I15" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="114">
-        <v>1733790.85</v>
-      </c>
-      <c r="F16" s="77">
-        <v>1733790.85</v>
-      </c>
-      <c r="G16" s="77"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="114">
-        <v>1733790.85</v>
-      </c>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91">
-        <v>468387.91</v>
-      </c>
-      <c r="H17" s="111"/>
-      <c r="I17" s="93" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="74" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="115" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="114">
-        <v>3488673.6</v>
-      </c>
-      <c r="F18" s="77">
-        <v>290722.8</v>
-      </c>
-      <c r="G18" s="77"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="74" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="81" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="116" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="74" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="115" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="114">
-        <v>3488673.6</v>
-      </c>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91">
-        <v>290722.8</v>
-      </c>
-      <c r="H19" s="111"/>
-      <c r="I19" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="L19" s="117" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="97" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="109">
-        <v>711963.26</v>
-      </c>
-      <c r="F20" s="110">
-        <v>100000</v>
-      </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="97" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="109">
-        <v>711963.26</v>
-      </c>
-      <c r="F21" s="91"/>
-      <c r="G21" s="91">
-        <v>100000</v>
-      </c>
-      <c r="H21" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="M21" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="119" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="120" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="121">
-        <v>125572.08</v>
-      </c>
-      <c r="F22" s="121">
-        <v>125572.08</v>
-      </c>
-      <c r="G22" s="122"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="106" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="L22" s="117" t="s">
-        <v>60</v>
-      </c>
-      <c r="M22" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="N22" s="123" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="107" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="110">
-        <v>3056166.2</v>
-      </c>
-      <c r="F23" s="110">
-        <v>100000</v>
-      </c>
-      <c r="G23" s="101"/>
-      <c r="H23" s="102"/>
-      <c r="I23" s="97" t="s">
-        <v>66</v>
-      </c>
-      <c r="J23" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L23" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="M23" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="107" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="110">
-        <v>3056166.2</v>
-      </c>
-      <c r="F24" s="91"/>
-      <c r="G24" s="121">
-        <v>100000</v>
-      </c>
-      <c r="H24" s="111"/>
-      <c r="I24" s="93" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K24" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L24" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="M24" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="N24" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="114">
-        <v>184935.72</v>
-      </c>
-      <c r="F25" s="77">
-        <v>184935.72</v>
-      </c>
-      <c r="G25" s="77"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="M25" s="124" t="s">
-        <v>73</v>
-      </c>
-      <c r="N25" s="125" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="114">
-        <v>184935.72</v>
-      </c>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91">
-        <v>184935.72</v>
-      </c>
-      <c r="H26" s="126" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="J26" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K26" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="L26" s="94" t="s">
-        <v>72</v>
-      </c>
-      <c r="M26" s="127" t="s">
-        <v>73</v>
-      </c>
-      <c r="N26" s="128" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="129" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="130" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="129" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="131" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132">
-        <v>320000</v>
-      </c>
-      <c r="G27" s="132"/>
-      <c r="H27" s="133"/>
-      <c r="I27" s="133" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="134" t="s">
-        <v>81</v>
-      </c>
-      <c r="L27" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="M27" s="127" t="s">
-        <v>73</v>
-      </c>
-      <c r="N27" s="128" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="135" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="136" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="135" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="137" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="138">
-        <v>68717.429999999993</v>
-      </c>
-      <c r="F28" s="138">
-        <v>68717.429999999993</v>
-      </c>
-      <c r="G28" s="138"/>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139" t="s">
-        <v>87</v>
-      </c>
-      <c r="J28" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="L28" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="M28" s="127" t="s">
-        <v>73</v>
-      </c>
-      <c r="N28" s="128" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:N23" xr:uid="{80B109D0-669A-4E04-8027-327E3EF3F49B}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8677365D-A5F6-4364-8DC2-782CBAA81BEF}">
-  <dimension ref="A4:K11"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" style="141"/>
-    <col min="2" max="2" width="12.42578125" style="141" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" style="141" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="141" customWidth="1"/>
-    <col min="5" max="5" width="9" style="141" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="141" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="141" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="141" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="141" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="141"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="163" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="163"/>
-      <c r="D4" s="163" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="151" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="151"/>
-    </row>
-    <row r="6" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="164" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-    </row>
-    <row r="7" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="166" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="167" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
-      <c r="J7" s="168"/>
-    </row>
-    <row r="8" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="157" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="144" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="144"/>
-      <c r="D8" s="145" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="149" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="149"/>
-      <c r="G8" s="145" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="145"/>
-      <c r="I8" s="156" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="158" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="155" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="147" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="150" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="150"/>
-      <c r="G9" s="152" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="153"/>
-      <c r="I9" s="148">
-        <v>271269.96000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="143"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="160"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="162" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="162"/>
-      <c r="G10" s="159" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="160"/>
-      <c r="I10" s="161"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G11" s="154"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B6:I6"/>
-  </mergeCells>
-  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>